<commit_message>
Worked on excel file
</commit_message>
<xml_diff>
--- a/chart samples.xlsx
+++ b/chart samples.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Desktop\project 1(again\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E677E6D5-6724-4EA0-BCA4-6243B4DB841A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8DA93C-2DC0-4708-8A89-34B6F203ADFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{FD8502AA-DD07-4DDE-B28F-827F5A976675}"/>
+    <workbookView xWindow="-25410" yWindow="930" windowWidth="21600" windowHeight="12240" activeTab="1" xr2:uid="{FD8502AA-DD07-4DDE-B28F-827F5A976675}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -19,9 +19,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
-    <pivotCache cacheId="14" r:id="rId5"/>
-    <pivotCache cacheId="12" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Unemployment Rate in Florida</t>
-  </si>
-  <si>
-    <t>Private Housing Building Permits</t>
   </si>
   <si>
     <t>Mean House Income Growth</t>
@@ -119,6 +116,9 @@
   <si>
     <t>Sum of House Price CF</t>
   </si>
+  <si>
+    <t>Private Housing Building Permits for Florida</t>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +127,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -180,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -194,11 +194,12 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,7 +207,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -315,6 +316,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -371,6 +375,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -427,6 +434,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -483,6 +493,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -4321,6 +4334,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -9751,7 +9767,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38793D0B-4466-4D10-94C9-1439FC97013A}" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38793D0B-4466-4D10-94C9-1439FC97013A}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A164:C197" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField axis="axisRow" showAll="0">
@@ -9920,7 +9936,7 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="Sum of Mean Household Income" fld="1" baseField="0" baseItem="0" numFmtId="178"/>
+    <dataField name="Sum of Mean Household Income" fld="1" baseField="0" baseItem="0" numFmtId="165"/>
     <dataField name="Sum of House Price CF" fld="12" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
@@ -9961,7 +9977,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C976DF63-BF42-490E-9993-88428582EE34}" name="PivotTable4" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C976DF63-BF42-490E-9993-88428582EE34}" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A126:B159" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" showAll="0">
@@ -10154,7 +10170,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55F7D5EB-4503-4995-9060-94E8ECA0D43B}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55F7D5EB-4503-4995-9060-94E8ECA0D43B}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A88:C121" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField axis="axisRow" showAll="0">
@@ -10364,7 +10380,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B7CE4305-AA6A-4329-998B-28C9967A0CA3}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B7CE4305-AA6A-4329-998B-28C9967A0CA3}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A46:C79" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField axis="axisRow" showAll="0">
@@ -10592,7 +10608,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8576E019-F3CD-4000-95D1-0686B35E7CEF}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8576E019-F3CD-4000-95D1-0686B35E7CEF}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:E36" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
@@ -11124,37 +11140,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4BDC62-8EFF-4844-BF18-9FBC98BFBABB}">
   <dimension ref="A3:E197"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A158" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1989</v>
       </c>
@@ -11171,7 +11187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1990</v>
       </c>
@@ -11188,7 +11204,7 @@
         <v>-0.22172278642292001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1991</v>
       </c>
@@ -11205,7 +11221,7 @@
         <v>-0.12008729192042226</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1992</v>
       </c>
@@ -11222,7 +11238,7 @@
         <v>0.16488827878969664</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>1993</v>
       </c>
@@ -11239,7 +11255,7 @@
         <v>0.14755383155014773</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1994</v>
       </c>
@@ -11256,7 +11272,7 @@
         <v>-1.2206848261306982E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1995</v>
       </c>
@@ -11273,7 +11289,7 @@
         <v>-0.11325475924830457</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1996</v>
       </c>
@@ -11290,7 +11306,7 @@
         <v>5.8188711854340311E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1997</v>
       </c>
@@ -11307,7 +11323,7 @@
         <v>-2.8887665286122678E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1998</v>
       </c>
@@ -11324,7 +11340,7 @@
         <v>7.6952832176879885E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1999</v>
       </c>
@@ -11341,7 +11357,7 @@
         <v>7.2290245950572096E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2000</v>
       </c>
@@ -11358,7 +11374,7 @@
         <v>-8.962016251523236E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>2001</v>
       </c>
@@ -11375,7 +11391,7 @@
         <v>0.12878115071456386</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>2002</v>
       </c>
@@ -11392,7 +11408,7 @@
         <v>9.9395870525688629E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>2003</v>
       </c>
@@ -11409,7 +11425,7 @@
         <v>0.18503783929990245</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2004</v>
       </c>
@@ -11426,7 +11442,7 @@
         <v>0.17346020092123249</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>2005</v>
       </c>
@@ -11443,7 +11459,7 @@
         <v>0.1540234139146244</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>2006</v>
       </c>
@@ -11460,7 +11476,7 @@
         <v>-0.27796869458551865</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>2007</v>
       </c>
@@ -11477,7 +11493,7 @@
         <v>-0.5112644833413712</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2008</v>
       </c>
@@ -11494,7 +11510,7 @@
         <v>-0.45533396907002782</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2009</v>
       </c>
@@ -11511,7 +11527,7 @@
         <v>-0.29895256074538695</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>2010</v>
       </c>
@@ -11528,7 +11544,7 @@
         <v>0.114681329754428</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>2011</v>
       </c>
@@ -11545,7 +11561,7 @@
         <v>3.2761590074890282E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>2012</v>
       </c>
@@ -11562,7 +11578,7 @@
         <v>0.33474438785134875</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>2013</v>
       </c>
@@ -11579,7 +11595,7 @@
         <v>0.30924262382198819</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>2014</v>
       </c>
@@ -11596,7 +11612,7 @@
         <v>1.3685942276801781E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>2015</v>
       </c>
@@ -11613,7 +11629,7 @@
         <v>0.16639085013258373</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>2016</v>
       </c>
@@ -11630,7 +11646,7 @@
         <v>0.12589155610092803</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>2017</v>
       </c>
@@ -11647,7 +11663,7 @@
         <v>0.12458379353239879</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>2018</v>
       </c>
@@ -11664,7 +11680,7 @@
         <v>0.1401678980439777</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>2019</v>
       </c>
@@ -11681,7 +11697,7 @@
         <v>4.7016844403349911E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>2020</v>
       </c>
@@ -11698,9 +11714,9 @@
         <v>0.1696614960858219</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="6">
         <v>1.0246726917803126</v>
@@ -11715,18 +11731,18 @@
         <v>0.81675851140077171</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>1989</v>
       </c>
@@ -11737,7 +11753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>1990</v>
       </c>
@@ -11748,7 +11764,7 @@
         <v>6.2300000000000001E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>1991</v>
       </c>
@@ -11759,7 +11775,7 @@
         <v>7.6399999999999996E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>1992</v>
       </c>
@@ -11770,7 +11786,7 @@
         <v>8.3699999999999997E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>1993</v>
       </c>
@@ -11781,7 +11797,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>1994</v>
       </c>
@@ -11792,7 +11808,7 @@
         <v>6.4799999999999996E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>1995</v>
       </c>
@@ -11803,7 +11819,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>1996</v>
       </c>
@@ -11814,7 +11830,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>1997</v>
       </c>
@@ -11825,7 +11841,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>1998</v>
       </c>
@@ -11836,7 +11852,7 @@
         <v>4.4499999999999998E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>1999</v>
       </c>
@@ -11847,7 +11863,7 @@
         <v>3.9300000000000002E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>2000</v>
       </c>
@@ -11858,7 +11874,7 @@
         <v>3.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>2001</v>
       </c>
@@ -11869,7 +11885,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>2002</v>
       </c>
@@ -11880,7 +11896,7 @@
         <v>4.9599999999999998E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>2003</v>
       </c>
@@ -11891,7 +11907,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>2004</v>
       </c>
@@ -11902,7 +11918,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>2005</v>
       </c>
@@ -11913,7 +11929,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>2006</v>
       </c>
@@ -11924,7 +11940,7 @@
         <v>2.47E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>2007</v>
       </c>
@@ -11935,7 +11951,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>2008</v>
       </c>
@@ -11946,7 +11962,7 @@
         <v>5.6899999999999999E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>2009</v>
       </c>
@@ -11957,7 +11973,7 @@
         <v>9.5600000000000004E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>2010</v>
       </c>
@@ -11968,7 +11984,7 @@
         <v>0.1082</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>2011</v>
       </c>
@@ -11979,7 +11995,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>2012</v>
       </c>
@@ -11990,7 +12006,7 @@
         <v>8.6699999999999999E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>2013</v>
       </c>
@@ -12001,7 +12017,7 @@
         <v>7.5300000000000006E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>2014</v>
       </c>
@@ -12012,7 +12028,7 @@
         <v>6.4299999999999996E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>2015</v>
       </c>
@@ -12023,7 +12039,7 @@
         <v>5.5199999999999999E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>2016</v>
       </c>
@@ -12034,7 +12050,7 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>2017</v>
       </c>
@@ -12045,7 +12061,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>2018</v>
       </c>
@@ -12056,7 +12072,7 @@
         <v>3.6499999999999998E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>2019</v>
       </c>
@@ -12067,7 +12083,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>2020</v>
       </c>
@@ -12078,9 +12094,9 @@
         <v>8.1699999999999995E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B79" s="6">
         <v>1.0246726917803126</v>
@@ -12089,18 +12105,18 @@
         <v>1.7881999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" t="s">
         <v>19</v>
       </c>
-      <c r="C88" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>1989</v>
       </c>
@@ -12111,7 +12127,7 @@
         <v>93.76</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>1990</v>
       </c>
@@ -12122,7 +12138,7 @@
         <v>96.01</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>1991</v>
       </c>
@@ -12133,7 +12149,7 @@
         <v>97.77</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>1992</v>
       </c>
@@ -12144,7 +12160,7 @@
         <v>99.88</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>1993</v>
       </c>
@@ -12155,7 +12171,7 @@
         <v>101.66</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>1994</v>
       </c>
@@ -12166,7 +12182,7 @@
         <v>100.86</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>1995</v>
       </c>
@@ -12177,7 +12193,7 @@
         <v>101.79</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>1996</v>
       </c>
@@ -12188,7 +12204,7 @@
         <v>104.4</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>1997</v>
       </c>
@@ -12199,7 +12215,7 @@
         <v>107.05</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>1998</v>
       </c>
@@ -12210,7 +12226,7 @@
         <v>112.03</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>1999</v>
       </c>
@@ -12221,7 +12237,7 @@
         <v>116.94</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>2000</v>
       </c>
@@ -12232,7 +12248,7 @@
         <v>124.64</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>2001</v>
       </c>
@@ -12243,7 +12259,7 @@
         <v>135.26</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>2002</v>
       </c>
@@ -12254,7 +12270,7 @@
         <v>145.37</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>2003</v>
       </c>
@@ -12265,7 +12281,7 @@
         <v>156.43</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>2004</v>
       </c>
@@ -12276,7 +12292,7 @@
         <v>177.67</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>2005</v>
       </c>
@@ -12287,7 +12303,7 @@
         <v>225.98</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>2006</v>
       </c>
@@ -12298,7 +12314,7 @@
         <v>272.79000000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>2007</v>
       </c>
@@ -12309,7 +12325,7 @@
         <v>272.98</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>2008</v>
       </c>
@@ -12320,7 +12336,7 @@
         <v>229.96</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>2009</v>
       </c>
@@ -12331,7 +12347,7 @@
         <v>190.69</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>2010</v>
       </c>
@@ -12342,7 +12358,7 @@
         <v>164.34</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>2011</v>
       </c>
@@ -12353,7 +12369,7 @@
         <v>149.32</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>2012</v>
       </c>
@@ -12364,7 +12380,7 @@
         <v>146.56</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>2013</v>
       </c>
@@ -12375,7 +12391,7 @@
         <v>161.13</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>2014</v>
       </c>
@@ -12386,7 +12402,7 @@
         <v>178.24</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>2015</v>
       </c>
@@ -12397,7 +12413,7 @@
         <v>193.82</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>2016</v>
       </c>
@@ -12408,7 +12424,7 @@
         <v>210.81</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>2017</v>
       </c>
@@ -12419,7 +12435,7 @@
         <v>231.24</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>2018</v>
       </c>
@@ -12430,7 +12446,7 @@
         <v>251.02</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>2019</v>
       </c>
@@ -12441,7 +12457,7 @@
         <v>266.79000000000002</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>2020</v>
       </c>
@@ -12452,9 +12468,9 @@
         <v>282.08</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B121" s="7">
         <v>9179.6400000000012</v>
@@ -12463,15 +12479,15 @@
         <v>5299.27</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B126" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>1989</v>
       </c>
@@ -12479,7 +12495,7 @@
         <v>5.0269925896120444</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>1990</v>
       </c>
@@ -12487,7 +12503,7 @@
         <v>5.0642511757302779</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>1991</v>
       </c>
@@ -12495,7 +12511,7 @@
         <v>5.1775364732529479</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>1992</v>
       </c>
@@ -12503,7 +12519,7 @@
         <v>5.0644158151932475</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>1993</v>
       </c>
@@ -12511,7 +12527,7 @@
         <v>5.113415627545586</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>1994</v>
       </c>
@@ -12519,7 +12535,7 @@
         <v>5.0022797045502907</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>1995</v>
       </c>
@@ -12527,7 +12543,7 @@
         <v>4.8624091381100722</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>1996</v>
       </c>
@@ -12535,7 +12551,7 @@
         <v>4.6842389835090561</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>1997</v>
       </c>
@@ -12543,7 +12559,7 @@
         <v>4.5327793637846652</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>1998</v>
       </c>
@@ -12551,7 +12567,7 @@
         <v>4.393254192575843</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
         <v>1999</v>
       </c>
@@ -12559,7 +12575,7 @@
         <v>4.0744792762465813</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>2000</v>
       </c>
@@ -12567,7 +12583,7 @@
         <v>4.0857622764548962</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>2001</v>
       </c>
@@ -12575,7 +12591,7 @@
         <v>4.7173804780876498</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>2002</v>
       </c>
@@ -12583,7 +12599,7 @@
         <v>5.2682926829268295</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
         <v>2003</v>
       </c>
@@ -12591,7 +12607,7 @@
         <v>5.7263314526629054</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>2004</v>
       </c>
@@ -12599,7 +12615,7 @@
         <v>6.018305788186467</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>2005</v>
       </c>
@@ -12607,7 +12623,7 @@
         <v>6.7534851416381407</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>2006</v>
       </c>
@@ -12615,7 +12631,7 @@
         <v>7.5019424403393327</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
         <v>2007</v>
       </c>
@@ -12623,7 +12639,7 @@
         <v>7.9431890652739714</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>2008</v>
       </c>
@@ -12631,7 +12647,7 @@
         <v>6.8382984818103694</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="5">
         <v>2009</v>
       </c>
@@ -12639,7 +12655,7 @@
         <v>6.3695613880570727</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>2010</v>
       </c>
@@ -12647,7 +12663,7 @@
         <v>5.7672830055352726</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="5">
         <v>2011</v>
       </c>
@@ -12655,7 +12671,7 @@
         <v>5.148250023712416</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>2012</v>
       </c>
@@ -12663,7 +12679,7 @@
         <v>4.4604471195184869</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <v>2013</v>
       </c>
@@ -12671,7 +12687,7 @@
         <v>4.9599373968664411</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>2014</v>
       </c>
@@ -12679,7 +12695,7 @@
         <v>4.9874015994491137</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="5">
         <v>2015</v>
       </c>
@@ -12687,7 +12703,7 @@
         <v>5.2291607204554671</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>2016</v>
       </c>
@@ -12695,7 +12711,7 @@
         <v>5.8586138858058945</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>2017</v>
       </c>
@@ -12703,7 +12719,7 @@
         <v>5.8048176497073394</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>2018</v>
       </c>
@@ -12711,7 +12727,7 @@
         <v>5.7723957723957726</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
         <v>2019</v>
       </c>
@@ -12719,7 +12735,7 @@
         <v>6.3540467711140298</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>2020</v>
       </c>
@@ -12727,26 +12743,26 @@
         <v>6.4195321652484001</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B159" s="7">
         <v>174.98048764535687</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B164" t="s">
+        <v>22</v>
+      </c>
+      <c r="C164" t="s">
         <v>23</v>
       </c>
-      <c r="C164" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
         <v>1989</v>
       </c>
@@ -12757,7 +12773,7 @@
         <v>93760</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>1990</v>
       </c>
@@ -12768,7 +12784,7 @@
         <v>96010</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
         <v>1991</v>
       </c>
@@ -12779,7 +12795,7 @@
         <v>97770</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>1992</v>
       </c>
@@ -12790,7 +12806,7 @@
         <v>99880</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
         <v>1993</v>
       </c>
@@ -12801,7 +12817,7 @@
         <v>101660</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
         <v>1994</v>
       </c>
@@ -12812,7 +12828,7 @@
         <v>100860</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="5">
         <v>1995</v>
       </c>
@@ -12823,7 +12839,7 @@
         <v>101790</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="5">
         <v>1996</v>
       </c>
@@ -12834,7 +12850,7 @@
         <v>104400</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="5">
         <v>1997</v>
       </c>
@@ -12845,7 +12861,7 @@
         <v>107050</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>1998</v>
       </c>
@@ -12856,7 +12872,7 @@
         <v>112030</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="5">
         <v>1999</v>
       </c>
@@ -12867,7 +12883,7 @@
         <v>116940</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>2000</v>
       </c>
@@ -12878,7 +12894,7 @@
         <v>124640</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="5">
         <v>2001</v>
       </c>
@@ -12889,7 +12905,7 @@
         <v>135260</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="5">
         <v>2002</v>
       </c>
@@ -12900,7 +12916,7 @@
         <v>145370</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="5">
         <v>2003</v>
       </c>
@@ -12911,7 +12927,7 @@
         <v>156430</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="5">
         <v>2004</v>
       </c>
@@ -12922,7 +12938,7 @@
         <v>177670</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="5">
         <v>2005</v>
       </c>
@@ -12933,7 +12949,7 @@
         <v>225980</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="5">
         <v>2006</v>
       </c>
@@ -12944,7 +12960,7 @@
         <v>272790</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="5">
         <v>2007</v>
       </c>
@@ -12955,7 +12971,7 @@
         <v>272980</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="5">
         <v>2008</v>
       </c>
@@ -12966,7 +12982,7 @@
         <v>229960</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="5">
         <v>2009</v>
       </c>
@@ -12977,7 +12993,7 @@
         <v>190690</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="5">
         <v>2010</v>
       </c>
@@ -12988,7 +13004,7 @@
         <v>164340</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="5">
         <v>2011</v>
       </c>
@@ -12999,7 +13015,7 @@
         <v>149320</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="5">
         <v>2012</v>
       </c>
@@ -13010,7 +13026,7 @@
         <v>146560</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="5">
         <v>2013</v>
       </c>
@@ -13021,7 +13037,7 @@
         <v>161130</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="5">
         <v>2014</v>
       </c>
@@ -13032,7 +13048,7 @@
         <v>178240</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="5">
         <v>2015</v>
       </c>
@@ -13043,7 +13059,7 @@
         <v>193820</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="5">
         <v>2016</v>
       </c>
@@ -13054,7 +13070,7 @@
         <v>210810</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="5">
         <v>2017</v>
       </c>
@@ -13065,7 +13081,7 @@
         <v>231240</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="5">
         <v>2018</v>
       </c>
@@ -13076,7 +13092,7 @@
         <v>251020</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="5">
         <v>2019</v>
       </c>
@@ -13087,7 +13103,7 @@
         <v>266790</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="5">
         <v>2020</v>
       </c>
@@ -13098,9 +13114,9 @@
         <v>282080</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B197" s="11">
         <v>1642243</v>
@@ -13117,31 +13133,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AC9897-AF76-4A71-8BA3-6987AD675F07}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13161,31 +13178,31 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1989</v>
       </c>
@@ -13230,7 +13247,7 @@
         <v>5.0269925896120444</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1990</v>
       </c>
@@ -13280,7 +13297,7 @@
         <v>5.0642511757302779</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1991</v>
       </c>
@@ -13307,30 +13324,30 @@
         <v>-5.6964959925813073E-3</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I33" si="1">(C4-C3)/C3</f>
+        <f t="shared" ref="I4:I35" si="1">(C4-C3)/C3</f>
         <v>1.6545680465633386E-2</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" ref="J4:J33" si="2">(D4-D3)/D3</f>
+        <f t="shared" ref="J4:J35" si="2">(D4-D3)/D3</f>
         <v>1.8331423810019693E-2</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K33" si="3">(G4-G3)/G3</f>
+        <f t="shared" ref="K4:K35" si="3">(G4-G3)/G3</f>
         <v>-0.12008729192042226</v>
       </c>
       <c r="L4" s="8">
         <v>7.6399999999999996E-2</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:M33" si="4">(G4-G3)/G3</f>
+        <f t="shared" ref="M4:M35" si="4">(G4-G3)/G3</f>
         <v>-0.12008729192042226</v>
       </c>
       <c r="N4" s="10">
-        <f t="shared" ref="N4:N33" si="5">(C4*1000)/B4</f>
+        <f t="shared" ref="N4:N35" si="5">(C4*1000)/B4</f>
         <v>5.1775364732529479</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1992</v>
       </c>
@@ -13380,7 +13397,7 @@
         <v>5.0644158151932475</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1993</v>
       </c>
@@ -13430,7 +13447,7 @@
         <v>5.113415627545586</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1994</v>
       </c>
@@ -13480,7 +13497,7 @@
         <v>5.0022797045502907</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1995</v>
       </c>
@@ -13530,7 +13547,7 @@
         <v>4.8624091381100722</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1996</v>
       </c>
@@ -13580,7 +13597,7 @@
         <v>4.6842389835090561</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1997</v>
       </c>
@@ -13630,7 +13647,7 @@
         <v>4.5327793637846652</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1998</v>
       </c>
@@ -13680,7 +13697,7 @@
         <v>4.393254192575843</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1999</v>
       </c>
@@ -13730,7 +13747,7 @@
         <v>4.0744792762465813</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2000</v>
       </c>
@@ -13780,7 +13797,7 @@
         <v>4.0857622764548962</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2001</v>
       </c>
@@ -13830,7 +13847,7 @@
         <v>4.7173804780876498</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2002</v>
       </c>
@@ -13880,7 +13897,7 @@
         <v>5.2682926829268295</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -13930,7 +13947,7 @@
         <v>5.7263314526629054</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -13980,7 +13997,7 @@
         <v>6.018305788186467</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2005</v>
       </c>
@@ -14030,7 +14047,7 @@
         <v>6.7534851416381407</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -14080,7 +14097,7 @@
         <v>7.5019424403393327</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2007</v>
       </c>
@@ -14130,7 +14147,7 @@
         <v>7.9431890652739714</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2008</v>
       </c>
@@ -14180,7 +14197,7 @@
         <v>6.8382984818103694</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -14230,7 +14247,7 @@
         <v>6.3695613880570727</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -14280,7 +14297,7 @@
         <v>5.7672830055352726</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -14330,7 +14347,7 @@
         <v>5.148250023712416</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2012</v>
       </c>
@@ -14380,7 +14397,7 @@
         <v>4.4604471195184869</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2013</v>
       </c>
@@ -14430,7 +14447,7 @@
         <v>4.9599373968664411</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2014</v>
       </c>
@@ -14480,7 +14497,7 @@
         <v>4.9874015994491137</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2015</v>
       </c>
@@ -14530,7 +14547,7 @@
         <v>5.2291607204554671</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2016</v>
       </c>
@@ -14580,7 +14597,7 @@
         <v>5.8586138858058945</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2017</v>
       </c>
@@ -14630,7 +14647,7 @@
         <v>5.8048176497073394</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2018</v>
       </c>
@@ -14653,7 +14670,7 @@
         <v>7905.89</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="0"/>
+        <f>(B31-B30)/B30</f>
         <v>8.232496623142728E-2</v>
       </c>
       <c r="I31" s="2">
@@ -14680,7 +14697,7 @@
         <v>5.7723957723957726</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2019</v>
       </c>
@@ -14730,7 +14747,7 @@
         <v>6.3540467711140298</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -14753,7 +14770,7 @@
         <v>9681.99</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="0"/>
+        <f>(B33-B32)/B32</f>
         <v>5.1835502173353733E-2</v>
       </c>
       <c r="I33" s="2">
@@ -14780,18 +14797,111 @@
         <v>6.4195321652484001</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2021</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>61777</v>
+      </c>
+      <c r="C34">
+        <v>586.78</v>
+      </c>
+      <c r="D34">
+        <v>323.86</v>
+      </c>
+      <c r="E34">
+        <v>2.96</v>
+      </c>
+      <c r="F34">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G34" s="12">
+        <v>12050.67</v>
+      </c>
+      <c r="H34" s="2">
+        <f>(B34-B33)/B33</f>
+        <v>-0.20469379610438096</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>0.17673719041411812</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14811401020986964</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24464805272469817</v>
+      </c>
+      <c r="L34" s="8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="4"/>
+        <v>0.24464805272469817</v>
+      </c>
+      <c r="N34" s="10">
+        <f t="shared" si="5"/>
+        <v>9.4983569937031582</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2022</v>
       </c>
+      <c r="B35">
+        <v>69884</v>
+      </c>
+      <c r="C35">
+        <v>737.44</v>
+      </c>
+      <c r="D35">
+        <v>400.26</v>
+      </c>
+      <c r="E35">
+        <v>5.34</v>
+      </c>
+      <c r="F35">
+        <v>2.9</v>
+      </c>
+      <c r="G35">
+        <v>10748.45</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" ref="H34:H35" si="6">(B35-B34)/B34</f>
+        <v>0.13123006944332033</v>
+      </c>
+      <c r="I35" s="2">
+        <f>(C35-C34)/C34</f>
+        <v>0.25675721735573825</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="2"/>
+        <v>0.23590440313715796</v>
+      </c>
+      <c r="K35" s="2">
+        <f>(G35-G34)/G34</f>
+        <v>-0.10806204136367516</v>
+      </c>
+      <c r="L35" s="6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="4"/>
+        <v>-0.10806204136367516</v>
+      </c>
+      <c r="N35" s="10">
+        <f>(C35*1000)/B35</f>
+        <v>10.552343884150879</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L36" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M3:M33">
+  <conditionalFormatting sqref="M3:M35">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -14821,7 +14931,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M3:M33</xm:sqref>
+          <xm:sqref>M3:M35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -14837,7 +14947,7 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>